<commit_message>
(added) - completed script
</commit_message>
<xml_diff>
--- a/assets/design/FDM Destinationer.xlsx
+++ b/assets/design/FDM Destinationer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="97">
   <si>
     <t>Paris</t>
   </si>
@@ -238,9 +238,6 @@
     <t>EDI</t>
   </si>
   <si>
-    <t>FINDES IKKE PÅ FDM-TRAVEL</t>
-  </si>
-  <si>
     <t>ROM</t>
   </si>
   <si>
@@ -293,6 +290,27 @@
   </si>
   <si>
     <t>SFO</t>
+  </si>
+  <si>
+    <t>DUB</t>
+  </si>
+  <si>
+    <t>REK</t>
+  </si>
+  <si>
+    <t>MLA</t>
+  </si>
+  <si>
+    <t>VIE</t>
+  </si>
+  <si>
+    <t>STO</t>
+  </si>
+  <si>
+    <t>BUD</t>
+  </si>
+  <si>
+    <t>DXB</t>
   </si>
 </sst>
 </file>
@@ -349,8 +367,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -375,7 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -385,6 +407,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -394,6 +418,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1079,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1167,7 +1193,7 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1181,7 +1207,7 @@
         <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1195,7 +1221,7 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1204,7 +1230,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1213,7 +1239,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1222,7 +1248,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1236,7 +1262,7 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1250,7 +1276,7 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1264,7 +1290,7 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1273,7 +1299,7 @@
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1360,7 +1386,7 @@
         <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1374,7 +1400,7 @@
         <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1383,7 +1409,7 @@
         <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1397,7 +1423,7 @@
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1411,7 +1437,7 @@
         <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1420,7 +1446,7 @@
         <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1434,7 +1460,7 @@
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1443,7 +1469,7 @@
         <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1457,7 +1483,7 @@
         <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1471,7 +1497,7 @@
         <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1485,7 +1511,7 @@
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1494,7 +1520,7 @@
         <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1503,7 +1529,7 @@
         <v>29</v>
       </c>
       <c r="C54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1512,7 +1538,7 @@
         <v>34</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1521,7 +1547,7 @@
         <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>